<commit_message>
updated schematic and BOM
</commit_message>
<xml_diff>
--- a/hardware/BOM MyGateway-ESP32-ETH.xlsx
+++ b/hardware/BOM MyGateway-ESP32-ETH.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bernd\Documents\Documents\Projects\HomeAutomation\MyGateway-ESP32-ETH\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bernd\Documents\Documents\Projects\HomeAutomation\MyGateway-ESP32-ETH\hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8E6C358-EDB9-4B79-A8B9-416417DC5436}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F99E7DD-B05F-4BBD-9CAD-6B2E4EAE4246}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3491" yWindow="2731" windowWidth="26002" windowHeight="14671" activeTab="1" xr2:uid="{BB90B514-33F2-4300-972D-50807DD95B5E}"/>
+    <workbookView xWindow="22184" yWindow="1236" windowWidth="20867" windowHeight="14672" activeTab="2" xr2:uid="{BB90B514-33F2-4300-972D-50807DD95B5E}"/>
   </bookViews>
   <sheets>
-    <sheet name="ETH Gateway" sheetId="1" r:id="rId1"/>
+    <sheet name="ETH Gateway «P»" sheetId="1" r:id="rId1"/>
     <sheet name="WiFi Repeater" sheetId="2" r:id="rId2"/>
+    <sheet name="ETH Repeater «Q»" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="43">
   <si>
     <t>Price/lot</t>
   </si>
@@ -134,6 +135,27 @@
   </si>
   <si>
     <t>Pollin 94‑260240</t>
+  </si>
+  <si>
+    <t>Aliexpress "Enclosure Case Plastic Box Circuit Board Project 100x80x29mm, WHITE"</t>
+  </si>
+  <si>
+    <t>Reichelt "RAD 470/16"</t>
+  </si>
+  <si>
+    <t>Capacitor 470µF 16V radial</t>
+  </si>
+  <si>
+    <t>Capacitor 100µF 50V SMD 1206</t>
+  </si>
+  <si>
+    <t>Aliexpress "100pcs 1206 Ceramic Capacitor 50V SMD Thick Film Chip Multilayer 100uF"</t>
+  </si>
+  <si>
+    <t>Capacitor 100nF 50V SMD 1206</t>
+  </si>
+  <si>
+    <t>Aliexpress "100pcs 1206 SMD Chip Multilayer Ceramic Capacitor 100nF 50V"</t>
   </si>
 </sst>
 </file>
@@ -143,7 +165,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -170,6 +192,12 @@
       <i/>
       <sz val="11"/>
       <color theme="4"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -518,10 +546,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A42964D-AF54-4802-907C-91158FA879F8}">
-  <dimension ref="B2:H12"/>
+  <dimension ref="B2:H15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="C26" sqref="C26:C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -532,7 +560,7 @@
     <row r="2" spans="2:8" x14ac:dyDescent="0.25">
       <c r="G2" s="1">
         <f>SUM(G4:G21)</f>
-        <v>11.394650000000002</v>
+        <v>11.519350000000003</v>
       </c>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
@@ -569,7 +597,7 @@
         <v>1</v>
       </c>
       <c r="G4" s="3">
-        <f t="shared" ref="G4:G12" si="0">+F4*E4</f>
+        <f t="shared" ref="G4:G15" si="0">+F4*E4</f>
         <v>2.2000000000000002</v>
       </c>
       <c r="H4" t="s">
@@ -587,7 +615,7 @@
         <v>1</v>
       </c>
       <c r="E5" s="3">
-        <f t="shared" ref="E5:E12" si="1">+C5/D5</f>
+        <f t="shared" ref="E5:E15" si="1">+C5/D5</f>
         <v>1.56</v>
       </c>
       <c r="F5">
@@ -774,6 +802,81 @@
       </c>
       <c r="H12" t="s">
         <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="D13">
+        <v>10</v>
+      </c>
+      <c r="E13" s="3">
+        <f t="shared" si="1"/>
+        <v>0.09</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13" s="3">
+        <f t="shared" si="0"/>
+        <v>0.09</v>
+      </c>
+      <c r="H13" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="3">
+        <v>2.59</v>
+      </c>
+      <c r="D14">
+        <v>100</v>
+      </c>
+      <c r="E14" s="3">
+        <f t="shared" si="1"/>
+        <v>2.5899999999999999E-2</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14" s="3">
+        <f t="shared" si="0"/>
+        <v>2.5899999999999999E-2</v>
+      </c>
+      <c r="H14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" s="3">
+        <v>0.88</v>
+      </c>
+      <c r="D15">
+        <v>100</v>
+      </c>
+      <c r="E15" s="3">
+        <f t="shared" si="1"/>
+        <v>8.8000000000000005E-3</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15" s="3">
+        <f t="shared" si="0"/>
+        <v>8.8000000000000005E-3</v>
+      </c>
+      <c r="H15" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -785,7 +888,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADCF8B02-6EF5-489E-81FE-685C9DF1729A}">
   <dimension ref="B2:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="S21" sqref="S21"/>
     </sheetView>
   </sheetViews>
@@ -828,14 +931,14 @@
         <v>1</v>
       </c>
       <c r="E4" s="3">
-        <f t="shared" ref="E4:E12" si="0">+C4/D4</f>
+        <f t="shared" ref="E4:E11" si="0">+C4/D4</f>
         <v>6.95</v>
       </c>
       <c r="F4">
         <v>1</v>
       </c>
       <c r="G4" s="3">
-        <f t="shared" ref="G4:G12" si="1">+F4*E4</f>
+        <f t="shared" ref="G4:G11" si="1">+F4*E4</f>
         <v>6.95</v>
       </c>
       <c r="H4" t="s">
@@ -1025,4 +1128,320 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BA2196B-A5C4-4A36-8C0D-90477C45CBAA}">
+  <dimension ref="B2:H14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="26.25" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="G2" s="1">
+        <f>SUM(G4:G21)</f>
+        <v>11.270350000000002</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="3">
+        <v>1.69</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4" s="3">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4" s="3">
+        <f t="shared" ref="G4:G14" si="0">+F4*E4</f>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="H4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="3">
+        <v>1.56</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5" s="3">
+        <f t="shared" ref="E5:E14" si="1">+C5/D5</f>
+        <v>1.56</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5" s="3">
+        <f t="shared" si="0"/>
+        <v>1.56</v>
+      </c>
+      <c r="H5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="3">
+        <v>2.36</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6" s="3">
+        <f t="shared" si="1"/>
+        <v>2.36</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6" s="3">
+        <f t="shared" si="0"/>
+        <v>2.36</v>
+      </c>
+      <c r="H6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="3">
+        <v>1.83</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7" s="3">
+        <f t="shared" si="1"/>
+        <v>1.83</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7" s="3">
+        <f t="shared" si="0"/>
+        <v>1.83</v>
+      </c>
+      <c r="H7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="3">
+        <v>2.35</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8" s="3">
+        <f t="shared" si="1"/>
+        <v>2.35</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8" s="3">
+        <f t="shared" si="0"/>
+        <v>2.35</v>
+      </c>
+      <c r="H8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="3">
+        <v>2.79</v>
+      </c>
+      <c r="D9">
+        <v>400</v>
+      </c>
+      <c r="E9" s="3">
+        <f t="shared" si="1"/>
+        <v>6.9750000000000003E-3</v>
+      </c>
+      <c r="F9">
+        <v>14</v>
+      </c>
+      <c r="G9" s="3">
+        <f t="shared" si="0"/>
+        <v>9.7650000000000001E-2</v>
+      </c>
+      <c r="H9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="3">
+        <v>0.64</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10" s="3">
+        <f t="shared" si="1"/>
+        <v>0.64</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10" s="3">
+        <f t="shared" si="0"/>
+        <v>0.64</v>
+      </c>
+      <c r="H10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="3">
+        <v>1.08</v>
+      </c>
+      <c r="D11">
+        <v>10</v>
+      </c>
+      <c r="E11" s="3">
+        <f t="shared" si="1"/>
+        <v>0.10800000000000001</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11" s="3">
+        <f t="shared" si="0"/>
+        <v>0.10800000000000001</v>
+      </c>
+      <c r="H11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="D12">
+        <v>10</v>
+      </c>
+      <c r="E12" s="3">
+        <f t="shared" si="1"/>
+        <v>0.09</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12" s="3">
+        <f t="shared" si="0"/>
+        <v>0.09</v>
+      </c>
+      <c r="H12" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" s="3">
+        <v>2.59</v>
+      </c>
+      <c r="D13">
+        <v>100</v>
+      </c>
+      <c r="E13" s="3">
+        <f t="shared" si="1"/>
+        <v>2.5899999999999999E-2</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13" s="3">
+        <f t="shared" si="0"/>
+        <v>2.5899999999999999E-2</v>
+      </c>
+      <c r="H13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14" s="3">
+        <v>0.88</v>
+      </c>
+      <c r="D14">
+        <v>100</v>
+      </c>
+      <c r="E14" s="3">
+        <f t="shared" si="1"/>
+        <v>8.8000000000000005E-3</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14" s="3">
+        <f t="shared" si="0"/>
+        <v>8.8000000000000005E-3</v>
+      </c>
+      <c r="H14" t="s">
+        <v>42</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>